<commit_message>
Add images for README.md file
</commit_message>
<xml_diff>
--- a/Project_5 Data_Story_Telling/Data & Analysis/Data/Local_Election_Turkey_2024.xlsx
+++ b/Project_5 Data_Story_Telling/Data & Analysis/Data/Local_Election_Turkey_2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alerd\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alerd\Studying Plan\Data Analysis Daily\Project_5 Data_Story_Telling\Data &amp; Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F0A418-E27A-4AE1-A12E-CBE1CE459070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7267C1D-5572-4D39-B164-98A253C8BAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="599">
   <si>
     <t>CITY</t>
   </si>
@@ -1817,9 +1817,6 @@
   </si>
   <si>
     <t>Uğur İbrahim Altay</t>
-  </si>
-  <si>
-    <t>https://secim.hurriyet.com.tr/31-mart-2024-yerel-secimleri/secim-sonuclari/</t>
   </si>
 </sst>
 </file>
@@ -2212,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5596,14 +5593,9 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A86" s="5" t="s">
-        <v>599</v>
-      </c>
+      <c r="A86" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A86" r:id="rId1" xr:uid="{ED605EB4-75D0-485E-B7C7-49C13FD6CD37}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>